<commit_message>
GenTime and Input Parameters
</commit_message>
<xml_diff>
--- a/InputParameters.xlsx
+++ b/InputParameters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icromwell/Desktop/My Work/Lymphoma/DES Model/DLBCL_DES_COO/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE140E-A54A-4E46-BA62-3DD8C7E77839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="-105" windowWidth="18045" windowHeight="14265"/>
+    <workbookView xWindow="13820" yWindow="840" windowWidth="14340" windowHeight="14260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -13,10 +19,16 @@
     <sheet name="PrefCoeffs" sheetId="4" r:id="rId4"/>
     <sheet name="TestChars" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,13 +38,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Cromwell</author>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="1">
+    <comment ref="A16" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="1">
+    <comment ref="A17" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="1">
+    <comment ref="A19" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -160,12 +172,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -195,12 +207,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Cromwell</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -231,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="138">
   <si>
     <t>TypeNo</t>
   </si>
@@ -248,12 +260,6 @@
     <t>NatHist_prevOPLunder50m</t>
   </si>
   <si>
-    <t>Tx_recurrence_probSurgery</t>
-  </si>
-  <si>
-    <t>Tx_stageI_probSurgery</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -317,66 +323,21 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>ref</t>
   </si>
   <si>
     <t>Assumption</t>
   </si>
   <si>
-    <t>Sigma</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>cancerStage</t>
-  </si>
-  <si>
-    <t>tx_prim</t>
-  </si>
-  <si>
-    <t>tx_recur</t>
-  </si>
-  <si>
     <t>Tx_stageI_probSurgeryRT</t>
   </si>
   <si>
     <t>Tx_stageI_probOther</t>
   </si>
   <si>
-    <t>Retrospective cohort</t>
-  </si>
-  <si>
-    <t>Tx_recurrence_probNonsurgery</t>
-  </si>
-  <si>
-    <t>Tx_recurrence_probPalliative</t>
-  </si>
-  <si>
     <t>Speight (2008)</t>
   </si>
   <si>
-    <t>Tx_recurrence_probNoTx</t>
-  </si>
-  <si>
     <t>NatHist_timeStagefour_death80plusm</t>
   </si>
   <si>
@@ -389,27 +350,6 @@
     <t>Util_Well</t>
   </si>
   <si>
-    <t>Adv</t>
-  </si>
-  <si>
-    <t>Surgery</t>
-  </si>
-  <si>
-    <t>SurgeryRT</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Nonsurgery</t>
-  </si>
-  <si>
-    <t>Palliative</t>
-  </si>
-  <si>
-    <t>Notx</t>
-  </si>
-  <si>
     <t>Treatment - Stage I - Surgery</t>
   </si>
   <si>
@@ -473,18 +413,6 @@
     <t>Treatment - Palliative</t>
   </si>
   <si>
-    <t>Cost_TxPrim</t>
-  </si>
-  <si>
-    <t>Cost_Recur</t>
-  </si>
-  <si>
-    <t>Cost_2Recur</t>
-  </si>
-  <si>
-    <t>Cost_EoL</t>
-  </si>
-  <si>
     <t>Weighted average + SD from MSP oncology f/u code (33512)</t>
   </si>
   <si>
@@ -503,9 +431,6 @@
     <t>VarNo</t>
   </si>
   <si>
-    <t>PtPref_Test</t>
-  </si>
-  <si>
     <t>Pref_patient_invasiveness</t>
   </si>
   <si>
@@ -648,13 +573,97 @@
   </si>
   <si>
     <t>addspecificity</t>
+  </si>
+  <si>
+    <t>Tx_MaxCycle</t>
+  </si>
+  <si>
+    <t>Tx_TimeTreat</t>
+  </si>
+  <si>
+    <t>Folup_Time_AppInterval</t>
+  </si>
+  <si>
+    <t>SysP_Followup</t>
+  </si>
+  <si>
+    <t>Util_Remission</t>
+  </si>
+  <si>
+    <t>Util_EoL</t>
+  </si>
+  <si>
+    <t>ClinHist_AssignRecurrence</t>
+  </si>
+  <si>
+    <t>Util_FollowUp</t>
+  </si>
+  <si>
+    <t>Util_AdvEvent_Standard</t>
+  </si>
+  <si>
+    <t>Util_AdvEvent_GEP</t>
+  </si>
+  <si>
+    <t>Util_Treatment_Standard</t>
+  </si>
+  <si>
+    <t>Util_Treatment_GEP</t>
+  </si>
+  <si>
+    <t>SysP_Treatment</t>
+  </si>
+  <si>
+    <t>Tx_ProbAdverseEvent_Standard</t>
+  </si>
+  <si>
+    <t>Tx_ProbAdverseEvent_GEP</t>
+  </si>
+  <si>
+    <t>Tx_Tprob_CRtoRecur</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>GCB</t>
+  </si>
+  <si>
+    <t>Dhit</t>
+  </si>
+  <si>
+    <t>Undef</t>
+  </si>
+  <si>
+    <t>GenPop</t>
+  </si>
+  <si>
+    <t>Under60</t>
+  </si>
+  <si>
+    <t>Over60</t>
+  </si>
+  <si>
+    <t>Tx_Tprob_CRtoDeath</t>
+  </si>
+  <si>
+    <t>Tx_Tprob_RecurtoDeath</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,13 +704,6 @@
       <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -750,7 +752,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -758,40 +760,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFC1C1C1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,23 +1078,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1119,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1128,12 +1111,12 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1148,9 +1131,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1165,9 +1148,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1179,12 +1162,12 @@
         <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1196,12 +1179,12 @@
         <v>166</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1213,12 +1196,12 @@
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1230,97 +1213,100 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0.05</v>
+      </c>
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.05</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11">
         <v>2</v>
-      </c>
-      <c r="D9">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12">
-        <v>235</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>180</v>
+      </c>
+      <c r="G12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1331,13 +1317,10 @@
       <c r="D13">
         <v>26</v>
       </c>
-      <c r="F13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -1348,53 +1331,50 @@
       <c r="D14">
         <v>58</v>
       </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="3">
         <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>-3.1318000000000001</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="3">
         <v>0.25790000000000002</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="7">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3">
         <v>7</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="3">
         <v>0.13</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -1409,12 +1389,12 @@
         <v>0.01</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -1429,12 +1409,12 @@
         <v>0.22359999999999999</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -1449,14 +1429,14 @@
         <v>0.1</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:11">
+        <v>27</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1471,9 +1451,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1488,9 +1468,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1505,9 +1485,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1522,9 +1502,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>9</v>
@@ -1536,8 +1516,67 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.4</v>
+      </c>
+      <c r="D26">
+        <v>0.01</v>
+      </c>
+      <c r="G26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:K95">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K95">
     <sortCondition ref="B2:B95"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1547,7 +1586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -1555,16 +1594,16 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1578,519 +1617,519 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43.1</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>254.91</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>250.4</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>43.1</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>254.91</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>59.51</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>250.4</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>59.51</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="5">
         <v>9268.5499999999993</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>10758.64</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="5">
         <v>9268.5499999999993</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>10758.64</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="5">
         <v>21219</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="5">
         <v>17525.96</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>7630.33</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>9051.5499999999993</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>19299.16</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>25503.439999999999</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>26059.51</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>18567.71</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>10279.56</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>8660.23</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>38185.449999999997</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>40438.870000000003</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="5">
         <v>34925.65</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="5">
         <v>22256.47</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="5">
         <v>14848.61</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="5">
         <v>16238.45</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="5">
         <v>29262.14</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="5">
         <v>42730.52</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="5">
         <v>17066.59</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="5">
         <v>20314.990000000002</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="5">
         <v>20778.66</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="5">
         <v>31106.02</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="5">
         <v>11119.52</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="5">
         <v>8518</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="5">
         <v>16616.98</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="5">
         <v>27427.74</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="5">
         <v>20778.66</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="5">
         <v>31106.02</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="5">
         <v>17930.25</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="5">
         <v>21977.09</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>591.29</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="9">
-        <v>591.29</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="5">
         <v>154</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="5">
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>80.67</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9">
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
         <v>80.67</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9">
-        <v>80.67</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="5">
         <v>154</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="5">
         <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F28" t="str">
         <f>F25</f>
         <v>Weighted average + SD from MSP oncology f/u code (33512)</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="5">
         <v>0</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="5"/>
       <c r="E30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2099,28 +2138,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -2129,471 +2168,1444 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
       </c>
       <c r="E2">
-        <v>9.2415000000000003</v>
+        <v>-4.8614649999999999</v>
       </c>
       <c r="F2">
-        <v>6.9400000000000003E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.56226900000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
       </c>
       <c r="E3">
-        <v>1.0499000000000001</v>
+        <v>-0.5228583</v>
       </c>
       <c r="F3">
-        <v>4.7699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.1233935</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
       </c>
       <c r="E4">
-        <v>2.0000000000000001E-4</v>
+        <v>-3.7219159999999998</v>
       </c>
       <c r="F4">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0.98258809999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E5">
+        <v>-0.96361240000000004</v>
+      </c>
+      <c r="F5">
+        <v>0.32371250000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="E6">
-        <v>-7.4300000000000005E-2</v>
+        <v>-5.4284239999999997</v>
       </c>
       <c r="F6">
-        <v>7.1800000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.6997776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E7">
+        <v>-0.66112340000000003</v>
+      </c>
+      <c r="F7">
+        <v>0.17157069999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="E8">
-        <v>0.58540000000000003</v>
+        <v>-5.125019</v>
       </c>
       <c r="F8">
-        <v>8.3400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>1.07975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="E9">
-        <v>1.0161</v>
+        <v>-0.54901319999999998</v>
       </c>
       <c r="F9">
-        <v>9.5200000000000007E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.24004819999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E10">
+        <v>-4.8843170000000002</v>
+      </c>
+      <c r="F10">
+        <v>1.047987</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>126</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="E11">
-        <v>0.50549999999999995</v>
+        <v>-0.6201063</v>
       </c>
       <c r="F11">
-        <v>0.11509999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>0.25068610000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="E12">
-        <v>-0.52290000000000003</v>
+        <v>-3.7219159999999998</v>
       </c>
       <c r="F12">
-        <v>8.0699999999999994E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0.98258809999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3">
-        <v>10.9358</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.65749999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13">
+        <v>-0.96361240000000004</v>
+      </c>
+      <c r="F13">
+        <v>0.32371250000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.71389999999999998</v>
-      </c>
-      <c r="F14" s="3">
-        <v>9.1899999999999996E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14">
+        <v>-5.3335249999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.99185429999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3">
-        <v>-1.0500000000000001E-2</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15">
+        <v>-0.70301809999999998</v>
+      </c>
+      <c r="F15">
+        <v>0.25211929999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E16">
+        <v>-4.8696770000000003</v>
+      </c>
+      <c r="F16">
+        <v>1.522791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4">
-        <v>2.1100000000000001E-2</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0.27610000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E17">
+        <v>-0.65110840000000003</v>
+      </c>
+      <c r="F17">
+        <v>0.37036229999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
+        <v>134</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E18">
+        <v>-4.8604849999999997</v>
+      </c>
+      <c r="F18">
+        <v>0.66654230000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
+        <v>134</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="5">
-        <v>-0.47539999999999999</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0.29799999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E19">
+        <v>-0.47558</v>
+      </c>
+      <c r="F19">
+        <v>0.14039889999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="5">
-        <v>-0.3306</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0.37190000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E20">
+        <v>-3.7219159999999998</v>
+      </c>
+      <c r="F20">
+        <v>0.98258809999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
+        <v>134</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="5">
-        <v>-0.95179999999999998</v>
-      </c>
-      <c r="F21" s="6">
-        <v>0.58040000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E21">
+        <v>-0.96361240000000004</v>
+      </c>
+      <c r="F21">
+        <v>0.32371250000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>127</v>
       </c>
       <c r="E22">
-        <v>12.154999999999999</v>
+        <v>-4.8389689999999996</v>
       </c>
       <c r="F22">
-        <v>2.2355999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0.70690160000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" t="s">
+        <v>128</v>
       </c>
       <c r="E23">
-        <v>0.90429999999999999</v>
+        <v>-0.75679850000000004</v>
       </c>
       <c r="F23">
-        <v>0.3221</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0.19084709999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
+        <v>134</v>
+      </c>
+      <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" t="s">
+        <v>127</v>
       </c>
       <c r="E24">
-        <v>-3.7699999999999997E-2</v>
+        <v>-5.4116799999999996</v>
       </c>
       <c r="F24">
-        <v>3.5799999999999998E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>1.5424359999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+        <v>134</v>
+      </c>
+      <c r="C25" t="s">
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>128</v>
+      </c>
+      <c r="E25">
+        <v>-0.4523102</v>
+      </c>
+      <c r="F25">
+        <v>0.31514569999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="E26">
-        <v>0.36919999999999997</v>
+        <v>-7.5961809999999996</v>
       </c>
       <c r="F26">
-        <v>1.0263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>1.4116519999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
       </c>
       <c r="E27">
-        <v>9.7909000000000006</v>
+        <v>-0.28306179999999997</v>
       </c>
       <c r="F27">
-        <v>4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>0.24249280000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>127</v>
       </c>
       <c r="E28">
-        <v>0.7419</v>
+        <v>-10.722340000000001</v>
       </c>
       <c r="F28">
-        <v>3.7999999999999999E-2</v>
+        <v>6.8431790000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29">
+        <v>1.65183E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.84597500000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30">
+        <v>-9.8273209999999995</v>
+      </c>
+      <c r="F30">
+        <v>1.49576</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31">
+        <v>1.4131700000000001E-2</v>
+      </c>
+      <c r="F31">
+        <v>0.1865637</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32">
+        <v>-9.6285810000000005</v>
+      </c>
+      <c r="F32">
+        <v>3.6240800000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33">
+        <v>-4.5154100000000003E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.4831473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34">
+        <v>-5.3542100000000001</v>
+      </c>
+      <c r="F34">
+        <v>1.811401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35">
+        <v>-1.0616540000000001</v>
+      </c>
+      <c r="F35">
+        <v>0.66370980000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36">
+        <v>-10.722340000000001</v>
+      </c>
+      <c r="F36">
+        <v>6.8431790000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37">
+        <v>1.65183E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.84597500000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38">
+        <v>-12.205679999999999</v>
+      </c>
+      <c r="F38">
+        <v>7.2096809999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39">
+        <v>3.87126E-2</v>
+      </c>
+      <c r="F39">
+        <v>0.8750618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40">
+        <v>-9.6285810000000005</v>
+      </c>
+      <c r="F40">
+        <v>3.6240800000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41">
+        <v>-4.5154100000000003E-2</v>
+      </c>
+      <c r="F41">
+        <v>0.4831473</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42">
+        <v>-8.7907849999999996</v>
+      </c>
+      <c r="F42">
+        <v>1.8740030000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43">
+        <v>-5.3880999999999998E-2</v>
+      </c>
+      <c r="F43">
+        <v>0.25437369999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44">
+        <v>-10.722340000000001</v>
+      </c>
+      <c r="F44">
+        <v>6.8431790000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45">
+        <v>1.65183E-2</v>
+      </c>
+      <c r="F45">
+        <v>0.84597500000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46">
+        <v>-9.4201750000000004</v>
+      </c>
+      <c r="F46">
+        <v>1.5367679999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47">
+        <v>2.1787299999999999E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.1904719</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48">
+        <v>-9.6285810000000005</v>
+      </c>
+      <c r="F48">
+        <v>3.6240800000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49">
+        <v>-4.5154100000000003E-2</v>
+      </c>
+      <c r="F49">
+        <v>0.4831473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50">
+        <v>-3.2747120000000001</v>
+      </c>
+      <c r="F50">
+        <v>0.45247939999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51">
+        <v>-0.63537929999999998</v>
+      </c>
+      <c r="F51">
+        <v>0.122891</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E52">
+        <v>-9.4869240000000001</v>
+      </c>
+      <c r="F52">
+        <v>2.7837209999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53">
+        <v>0.70038330000000004</v>
+      </c>
+      <c r="F53">
+        <v>0.27812809999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54">
+        <v>-3.1834349999999998</v>
+      </c>
+      <c r="F54">
+        <v>0.62189530000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55">
+        <v>-0.75665110000000002</v>
+      </c>
+      <c r="F55">
+        <v>0.1885936</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" t="s">
+        <v>127</v>
+      </c>
+      <c r="E56">
+        <v>-3.3841510000000001</v>
+      </c>
+      <c r="F56">
+        <v>0.85316999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" t="s">
+        <v>128</v>
+      </c>
+      <c r="E57">
+        <v>-0.58586269999999996</v>
+      </c>
+      <c r="F57">
+        <v>0.22330649999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" t="s">
+        <v>127</v>
+      </c>
+      <c r="E58">
+        <v>-3.3393130000000002</v>
+      </c>
+      <c r="F58">
+        <v>0.98982800000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59">
+        <v>-0.80166400000000004</v>
+      </c>
+      <c r="F59">
+        <v>0.29951870000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" t="s">
+        <v>127</v>
+      </c>
+      <c r="E60">
+        <v>-9.4869240000000001</v>
+      </c>
+      <c r="F60">
+        <v>2.7837209999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61">
+        <v>0.70038330000000004</v>
+      </c>
+      <c r="F61">
+        <v>0.27812809999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" t="s">
+        <v>127</v>
+      </c>
+      <c r="E62">
+        <v>-3.1833879999999999</v>
+      </c>
+      <c r="F62">
+        <v>0.92363510000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" t="s">
+        <v>128</v>
+      </c>
+      <c r="E63">
+        <v>-0.83449700000000004</v>
+      </c>
+      <c r="F63">
+        <v>0.28962919999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64">
+        <v>-3.6348850000000001</v>
+      </c>
+      <c r="F64">
+        <v>1.385478</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" t="s">
+        <v>128</v>
+      </c>
+      <c r="E65">
+        <v>-0.51855770000000001</v>
+      </c>
+      <c r="F65">
+        <v>0.34395890000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66">
+        <v>-3.3733050000000002</v>
+      </c>
+      <c r="F66">
+        <v>0.52197899999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E67">
+        <v>-0.53891429999999996</v>
+      </c>
+      <c r="F67">
+        <v>0.1329236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68">
+        <v>-9.4869240000000001</v>
+      </c>
+      <c r="F68">
+        <v>2.7837209999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69" t="s">
+        <v>128</v>
+      </c>
+      <c r="E69">
+        <v>0.70038330000000004</v>
+      </c>
+      <c r="F69">
+        <v>0.27812809999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" t="s">
+        <v>127</v>
+      </c>
+      <c r="E70">
+        <v>-3.5435949999999998</v>
+      </c>
+      <c r="F70">
+        <v>0.70051419999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71" t="s">
+        <v>128</v>
+      </c>
+      <c r="E71">
+        <v>-0.47834569999999998</v>
+      </c>
+      <c r="F71">
+        <v>0.1784395</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72">
+        <v>-3.2215929999999999</v>
+      </c>
+      <c r="F72">
+        <v>1.083429</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" t="s">
+        <v>128</v>
+      </c>
+      <c r="E73">
+        <v>-0.63080709999999995</v>
+      </c>
+      <c r="F73">
+        <v>0.29363230000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2603,32 +3615,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="3" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="3" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2640,38 +3652,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2683,18 +3695,18 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2706,15 +3718,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2726,18 +3738,18 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2749,18 +3761,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2772,18 +3784,18 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2795,35 +3807,35 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -2835,15 +3847,15 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -2855,38 +3867,38 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2898,18 +3910,18 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -2921,32 +3933,32 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -2958,18 +3970,18 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2981,18 +3993,18 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3004,35 +4016,35 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>105</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>134</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -3044,15 +4056,15 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -3070,163 +4082,163 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3235,12 +4247,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3249,12 +4261,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3263,12 +4275,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3277,12 +4289,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C13">
         <v>0</v>

</xml_diff>